<commit_message>
replace specific project code with generic
</commit_message>
<xml_diff>
--- a/Analysis/measures.xlsx
+++ b/Analysis/measures.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\MAA2016-15 Supporting the Social Investment Unit\Exemplar project\Analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NotBackedUp\local R dev\idi_exemplar_project\Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E674DE36-A7F1-4FD0-8DBE-88F57A128117}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21585" windowHeight="9015"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -158,9 +159,6 @@
     <t>[IDI_UserCode]</t>
   </si>
   <si>
-    <t>[DL-MAA2020-01]</t>
-  </si>
-  <si>
     <t>[IDI_Sandpit]</t>
   </si>
   <si>
@@ -228,12 +226,15 @@
   </si>
   <si>
     <t>Total taxable income</t>
+  </si>
+  <si>
+    <t>[DL-MAA20XX-YY]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
@@ -287,8 +288,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Comma 2" xfId="1"/>
-    <cellStyle name="Comma 2 2" xfId="2"/>
+    <cellStyle name="Comma 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Comma 2 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -566,10 +567,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -638,7 +641,7 @@
         <v>15</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>16</v>
@@ -673,7 +676,7 @@
         <v>15</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>16</v>
@@ -709,7 +712,7 @@
         <v>15</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>16</v>
@@ -745,7 +748,7 @@
         <v>15</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>16</v>
@@ -781,7 +784,7 @@
         <v>15</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>16</v>
@@ -817,7 +820,7 @@
         <v>15</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>16</v>
@@ -853,7 +856,7 @@
         <v>15</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>16</v>
@@ -889,7 +892,7 @@
         <v>15</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>16</v>
@@ -898,7 +901,7 @@
         <v>39</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>40</v>
@@ -912,31 +915,31 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>40</v>
@@ -945,36 +948,36 @@
         <v>0</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>17</v>
@@ -983,36 +986,36 @@
         <v>0</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J12" t="s">
         <v>17</v>
@@ -1021,45 +1024,45 @@
         <v>0</v>
       </c>
       <c r="L12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F13" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="H13" t="s">
         <v>64</v>
       </c>
-      <c r="H13" t="s">
-        <v>65</v>
-      </c>
       <c r="I13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K13" s="2" t="b">
         <v>0</v>
       </c>
       <c r="L13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>